<commit_message>
Update Calendário e Testes Firebase
Atualização do calendário após reunião
</commit_message>
<xml_diff>
--- a/Calendário TG.xlsx
+++ b/Calendário TG.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9743D6BE-9892-45E2-9EC0-2AD2A69379CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399ADC23-78EF-4793-A35B-12DA5810137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendário" sheetId="14" r:id="rId1"/>
@@ -93,7 +93,6 @@
     <definedName name="ValorDoInícioDaSemana">IF(InícioDaSemana="SEGUNDA-FEIRA",2,1)</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -109,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Anotações:</t>
   </si>
@@ -182,6 +181,39 @@
 &gt; Definição de target de acuracia;
 &gt; Revisar trabalho escrito;</t>
   </si>
+  <si>
+    <t>&gt; Definição de algoritmos a serem treinados (máximo 3) e a forma de sua implementação;
+&gt; Pesquisa de implementação do Firebase no python;
+&gt; Pequisa de relatório de treinamento no Tensorflow;
+&gt; Pesquisar ferramentas para treinamentos de modelos;
+&gt; Definição de target de acuracia;</t>
+  </si>
+  <si>
+    <t>Proxima semana:
+&gt; Revisar trabalho escrito;</t>
+  </si>
+  <si>
+    <t>&gt; Revisar trabalho escrito;</t>
+  </si>
+  <si>
+    <t>Proxima semana:
+&gt; Iniciar implementação Firebase
+&gt; Iniciar implementação Tensowflow
+&gt; Revisar trabalho escrito</t>
+  </si>
+  <si>
+    <t>&gt; Iniciar implementação Firebase
+&gt; Definição de método de uso Firebase
+&gt; Iniciar implementação Tensowboard
+&gt; Iniciar implementação Tensowflow
+&gt; Revisar trabalho escrito</t>
+  </si>
+  <si>
+    <t>Proxima semana:
+&gt; Iniciar Coleta de Dados e Baterias de Teste
+&gt; Definir padrão de relatório para as coletas
+&gt; Pesquisa de trabalhos relacionados</t>
+  </si>
 </sst>
 </file>
 
@@ -195,7 +227,7 @@
     <numFmt numFmtId="166" formatCode="dd"/>
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Trebuchet MS"/>
@@ -376,14 +408,6 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -399,7 +423,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -660,6 +684,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,22 +1056,19 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="5" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="37" borderId="6" xfId="6" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="38" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="39" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1065,7 +1092,7 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="40" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1077,8 +1104,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1086,11 +1113,11 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1124,6 +1151,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="47" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1552,10 +1582,10 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H168"/>
+  <dimension ref="A1:I168"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1563,26 +1593,26 @@
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="18.25" customWidth="1"/>
     <col min="3" max="7" width="17.625" customWidth="1"/>
-    <col min="8" max="8" width="23.75" customWidth="1"/>
-    <col min="9" max="11" width="17.5" customWidth="1"/>
+    <col min="8" max="9" width="37.5" customWidth="1"/>
+    <col min="10" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="2"/>
       <c r="B1" s="1">
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -1612,7 +1642,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <f t="array" aca="1" ref="B3:H3" ca="1">Dias+1+DATE(CalendárioAno1,CaléndárioMês1Opção,1)-WEEKDAY(DATE(CalendárioAno1,CaléndárioMês1Opção,1),DiaDaSemanaOpção)</f>
         <v>44620</v>
@@ -1642,7 +1672,7 @@
         <v>44626</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1651,7 +1681,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
         <f t="array" aca="1" ref="B5:H5" ca="1">Dias+8+DATE(CalendárioAno1,CaléndárioMês1Opção,1)-WEEKDAY(DATE(CalendárioAno1,CaléndárioMês1Opção,1),DiaDaSemanaOpção)</f>
         <v>44627</v>
@@ -1681,18 +1711,18 @@
         <v>44633</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="135" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="123.75" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <f t="array" aca="1" ref="B7:H7" ca="1">Dias+15+DATE(CalendárioAno1,CaléndárioMês1Opção,1)-WEEKDAY(DATE(CalendárioAno1,CaléndárioMês1Opção,1),DiaDaSemanaOpção)</f>
         <v>44634</v>
@@ -1722,16 +1752,21 @@
         <v>44640</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="101.25" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
         <f t="array" aca="1" ref="B9:H9" ca="1">Dias+22+DATE(CalendárioAno1,CaléndárioMês1Opção,1)-WEEKDAY(DATE(CalendárioAno1,CaléndárioMês1Opção,1),DiaDaSemanaOpção)</f>
         <v>44641</v>
@@ -1761,16 +1796,21 @@
         <v>44647</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="14"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B11" s="10">
         <f t="array" aca="1" ref="B11:H11" ca="1">Dias+29+DATE(CalendárioAno1,CaléndárioMês1Opção,1)-WEEKDAY(DATE(CalendárioAno1,CaléndárioMês1Opção,1),DiaDaSemanaOpção)</f>
         <v>44648</v>
@@ -1800,7 +1840,7 @@
         <v>44654</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1809,7 +1849,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
         <f t="array" aca="1" ref="B13:C13" ca="1">Dias+36+DATE(CalendárioAno1,CaléndárioMês1Opção,1)-WEEKDAY(DATE(CalendárioAno1,CaléndárioMês1Opção,1),DiaDaSemanaOpção)</f>
         <v>44655</v>
@@ -1826,32 +1866,32 @@
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
     </row>
-    <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-    </row>
-    <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C15" s="35" t="str">
+      <c r="C15" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1),"mmmm")</f>
         <v>abril</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="str">
         <f ca="1">UPPER(TEXT(B17,"dddd"))</f>
@@ -1882,7 +1922,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B17" s="10">
         <f t="array" aca="1" ref="B17:H17" ca="1">Dias+1+DATE(CalendárioAno2,CaléndárioMês2Opção,1)-WEEKDAY(DATE(CalendárioAno2,CaléndárioMês2Opção,1),DiaDaSemanaOpção)</f>
         <v>44648</v>
@@ -1912,16 +1952,21 @@
         <v>44654</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <f t="array" aca="1" ref="B19:H19" ca="1">Dias+8+DATE(CalendárioAno2,CaléndárioMês2Opção,1)-WEEKDAY(DATE(CalendárioAno2,CaléndárioMês2Opção,1),DiaDaSemanaOpção)</f>
         <v>44655</v>
@@ -1951,7 +1996,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1960,7 +2005,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <f t="array" aca="1" ref="B21:H21" ca="1">Dias+15+DATE(CalendárioAno2,CaléndárioMês2Opção,1)-WEEKDAY(DATE(CalendárioAno2,CaléndárioMês2Opção,1),DiaDaSemanaOpção)</f>
         <v>44662</v>
@@ -1990,7 +2035,7 @@
         <v>44668</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -2001,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B23" s="10">
         <f t="array" aca="1" ref="B23:H23" ca="1">Dias+22+DATE(CalendárioAno2,CaléndárioMês2Opção,1)-WEEKDAY(DATE(CalendárioAno2,CaléndárioMês2Opção,1),DiaDaSemanaOpção)</f>
         <v>44669</v>
@@ -2031,7 +2076,7 @@
         <v>44675</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -2040,7 +2085,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <f t="array" aca="1" ref="B25:H25" ca="1">Dias+29+DATE(CalendárioAno2,CaléndárioMês2Opção,1)-WEEKDAY(DATE(CalendárioAno2,CaléndárioMês2Opção,1),DiaDaSemanaOpção)</f>
         <v>44676</v>
@@ -2070,7 +2115,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2079,7 +2124,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="9"/>
     </row>
-    <row r="27" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <f t="array" aca="1" ref="B27:C27" ca="1">Dias+36+DATE(CalendárioAno2,CaléndárioMês2Opção,1)-WEEKDAY(DATE(CalendárioAno2,CaléndárioMês2Opção,1),DiaDaSemanaOpção)</f>
         <v>44683</v>
@@ -2088,40 +2133,40 @@
         <f ca="1"/>
         <v>44684</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-    </row>
-    <row r="28" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-    </row>
-    <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+    </row>
+    <row r="29" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A29" s="2"/>
       <c r="B29" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C29" s="35" t="str">
+      <c r="C29" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1),"mmmm")</f>
         <v>maio</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="str">
         <f t="shared" ref="B30:H30" ca="1" si="2">UPPER(TEXT(B31,"dddd"))</f>
@@ -2152,7 +2197,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <f t="array" aca="1" ref="B31:H31" ca="1">Dias+1+DATE(CalendárioAno3,CaléndárioMês3Opção,1)-WEEKDAY(DATE(CalendárioAno3,CaléndárioMês3Opção,1),DiaDaSemanaOpção)</f>
         <v>44676</v>
@@ -2182,7 +2227,7 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -2191,7 +2236,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
         <f t="array" aca="1" ref="B33:H33" ca="1">Dias+8+DATE(CalendárioAno3,CaléndárioMês3Opção,1)-WEEKDAY(DATE(CalendárioAno3,CaléndárioMês3Opção,1),DiaDaSemanaOpção)</f>
         <v>44683</v>
@@ -2221,7 +2266,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -2230,7 +2275,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B35" s="10">
         <f t="array" aca="1" ref="B35:H35" ca="1">Dias+15+DATE(CalendárioAno3,CaléndárioMês3Opção,1)-WEEKDAY(DATE(CalendárioAno3,CaléndárioMês3Opção,1),DiaDaSemanaOpção)</f>
         <v>44690</v>
@@ -2260,7 +2305,7 @@
         <v>44696</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -2269,7 +2314,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B37" s="10">
         <f t="array" aca="1" ref="B37:H37" ca="1">Dias+22+DATE(CalendárioAno3,CaléndárioMês3Opção,1)-WEEKDAY(DATE(CalendárioAno3,CaléndárioMês3Opção,1),DiaDaSemanaOpção)</f>
         <v>44697</v>
@@ -2299,7 +2344,7 @@
         <v>44703</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -2308,7 +2353,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B39" s="10">
         <f t="array" aca="1" ref="B39:H39" ca="1">Dias+29+DATE(CalendárioAno3,CaléndárioMês3Opção,1)-WEEKDAY(DATE(CalendárioAno3,CaléndárioMês3Opção,1),DiaDaSemanaOpção)</f>
         <v>44704</v>
@@ -2338,7 +2383,7 @@
         <v>44710</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -2347,7 +2392,7 @@
       <c r="G40" s="7"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B41" s="10">
         <f t="array" aca="1" ref="B41:C41" ca="1">Dias+36+DATE(CalendárioAno3,CaléndárioMês3Opção,1)-WEEKDAY(DATE(CalendárioAno3,CaléndárioMês3Opção,1),DiaDaSemanaOpção)</f>
         <v>44711</v>
@@ -2356,40 +2401,40 @@
         <f ca="1"/>
         <v>44712</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-    </row>
-    <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-    </row>
-    <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+    </row>
+    <row r="43" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A43" s="2"/>
       <c r="B43" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C43" s="35" t="str">
+      <c r="C43" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1),"mmmm")</f>
         <v>junho</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="str">
         <f t="shared" ref="B44:H44" ca="1" si="3">UPPER(TEXT(B45,"dddd"))</f>
@@ -2420,7 +2465,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B45" s="10">
         <f t="array" aca="1" ref="B45:H45" ca="1">Dias+1+DATE(CalendárioAno4,CaléndárioMês4Opção,1)-WEEKDAY(DATE(CalendárioAno4,CaléndárioMês4Opção,1),DiaDaSemanaOpção)</f>
         <v>44711</v>
@@ -2450,7 +2495,7 @@
         <v>44717</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -2460,7 +2505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B47" s="10">
         <f t="array" aca="1" ref="B47:H47" ca="1">Dias+8+DATE(CalendárioAno4,CaléndárioMês4Opção,1)-WEEKDAY(DATE(CalendárioAno4,CaléndárioMês4Opção,1),DiaDaSemanaOpção)</f>
         <v>44718</v>
@@ -2490,7 +2535,7 @@
         <v>44724</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="13"/>
       <c r="D48" s="7"/>
@@ -2501,7 +2546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B49" s="10">
         <f t="array" aca="1" ref="B49:H49" ca="1">Dias+15+DATE(CalendárioAno4,CaléndárioMês4Opção,1)-WEEKDAY(DATE(CalendárioAno4,CaléndárioMês4Opção,1),DiaDaSemanaOpção)</f>
         <v>44725</v>
@@ -2531,7 +2576,7 @@
         <v>44731</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B50" s="7"/>
       <c r="C50" s="13"/>
       <c r="D50" s="7"/>
@@ -2540,7 +2585,7 @@
       <c r="G50" s="7"/>
       <c r="H50" s="12"/>
     </row>
-    <row r="51" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B51" s="10">
         <f t="array" aca="1" ref="B51:H51" ca="1">Dias+22+DATE(CalendárioAno4,CaléndárioMês4Opção,1)-WEEKDAY(DATE(CalendárioAno4,CaléndárioMês4Opção,1),DiaDaSemanaOpção)</f>
         <v>44732</v>
@@ -2570,7 +2615,7 @@
         <v>44738</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B52" s="7"/>
       <c r="C52" s="13"/>
       <c r="D52" s="7"/>
@@ -2579,7 +2624,7 @@
       <c r="G52" s="7"/>
       <c r="H52" s="12"/>
     </row>
-    <row r="53" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B53" s="10">
         <f t="array" aca="1" ref="B53:H53" ca="1">Dias+29+DATE(CalendárioAno4,CaléndárioMês4Opção,1)-WEEKDAY(DATE(CalendárioAno4,CaléndárioMês4Opção,1),DiaDaSemanaOpção)</f>
         <v>44739</v>
@@ -2609,7 +2654,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
       <c r="C54" s="13"/>
       <c r="D54" s="7"/>
@@ -2617,7 +2662,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B55" s="10">
         <f t="array" aca="1" ref="B55:C55" ca="1">Dias+36+DATE(CalendárioAno4,CaléndárioMês4Opção,1)-WEEKDAY(DATE(CalendárioAno4,CaléndárioMês4Opção,1),DiaDaSemanaOpção)</f>
         <v>44746</v>
@@ -2626,40 +2671,40 @@
         <f ca="1"/>
         <v>44747</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D55" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-    </row>
-    <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="39"/>
-    </row>
-    <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+    </row>
+    <row r="57" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A57" s="2"/>
       <c r="B57" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C57" s="35" t="str">
+      <c r="C57" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1),"mmmm")</f>
         <v>julho</v>
       </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="4" t="str">
         <f t="shared" ref="B58:H58" ca="1" si="4">UPPER(TEXT(B59,"dddd"))</f>
@@ -2690,7 +2735,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B59" s="10">
         <f t="array" aca="1" ref="B59:H59" ca="1">Dias+1+DATE(CalendárioAno5,CaléndárioMês5Opção,1)-WEEKDAY(DATE(CalendárioAno5,CaléndárioMês5Opção,1),DiaDaSemanaOpção)</f>
         <v>44739</v>
@@ -2720,7 +2765,7 @@
         <v>44745</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -2729,7 +2774,7 @@
       <c r="G60" s="7"/>
       <c r="H60" s="15"/>
     </row>
-    <row r="61" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B61" s="10">
         <f t="array" aca="1" ref="B61:H61" ca="1">Dias+8+DATE(CalendárioAno5,CaléndárioMês5Opção,1)-WEEKDAY(DATE(CalendárioAno5,CaléndárioMês5Opção,1),DiaDaSemanaOpção)</f>
         <v>44746</v>
@@ -2759,7 +2804,7 @@
         <v>44752</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -2768,7 +2813,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="15"/>
     </row>
-    <row r="63" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B63" s="10">
         <f t="array" aca="1" ref="B63:H63" ca="1">Dias+15+DATE(CalendárioAno5,CaléndárioMês5Opção,1)-WEEKDAY(DATE(CalendárioAno5,CaléndárioMês5Opção,1),DiaDaSemanaOpção)</f>
         <v>44753</v>
@@ -2798,7 +2843,7 @@
         <v>44759</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -2807,7 +2852,7 @@
       <c r="G64" s="7"/>
       <c r="H64" s="15"/>
     </row>
-    <row r="65" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B65" s="10">
         <f t="array" aca="1" ref="B65:H65" ca="1">Dias+22+DATE(CalendárioAno5,CaléndárioMês5Opção,1)-WEEKDAY(DATE(CalendárioAno5,CaléndárioMês5Opção,1),DiaDaSemanaOpção)</f>
         <v>44760</v>
@@ -2837,7 +2882,7 @@
         <v>44766</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -2846,7 +2891,7 @@
       <c r="G66" s="7"/>
       <c r="H66" s="15"/>
     </row>
-    <row r="67" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B67" s="10">
         <f t="array" aca="1" ref="B67:H67" ca="1">Dias+29+DATE(CalendárioAno5,CaléndárioMês5Opção,1)-WEEKDAY(DATE(CalendárioAno5,CaléndárioMês5Opção,1),DiaDaSemanaOpção)</f>
         <v>44767</v>
@@ -2876,7 +2921,7 @@
         <v>44773</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -2885,7 +2930,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="9"/>
     </row>
-    <row r="69" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B69" s="10">
         <f t="array" aca="1" ref="B69:C69" ca="1">Dias+36+DATE(CalendárioAno5,CaléndárioMês5Opção,1)-WEEKDAY(DATE(CalendárioAno5,CaléndárioMês5Opção,1),DiaDaSemanaOpção)</f>
         <v>44774</v>
@@ -2894,40 +2939,40 @@
         <f ca="1"/>
         <v>44775</v>
       </c>
-      <c r="D69" s="36" t="s">
+      <c r="D69" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="37"/>
-    </row>
-    <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="39"/>
-    </row>
-    <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
+      <c r="H70" s="34"/>
+    </row>
+    <row r="71" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A71" s="2"/>
       <c r="B71" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C71" s="35" t="str">
+      <c r="C71" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1),"mmmm")</f>
         <v>agosto</v>
       </c>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="str">
         <f t="shared" ref="B72:H72" ca="1" si="5">UPPER(TEXT(B73,"dddd"))</f>
@@ -2958,7 +3003,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B73" s="10">
         <f t="array" aca="1" ref="B73:H73" ca="1">Dias+1+DATE(CalendárioAno6,CaléndárioMês6Opção,1)-WEEKDAY(DATE(CalendárioAno6,CaléndárioMês6Opção,1),DiaDaSemanaOpção)</f>
         <v>44774</v>
@@ -2988,7 +3033,7 @@
         <v>44780</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -2997,7 +3042,7 @@
       <c r="G74" s="7"/>
       <c r="H74" s="8"/>
     </row>
-    <row r="75" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B75" s="10">
         <f t="array" aca="1" ref="B75:H75" ca="1">Dias+8+DATE(CalendárioAno6,CaléndárioMês6Opção,1)-WEEKDAY(DATE(CalendárioAno6,CaléndárioMês6Opção,1),DiaDaSemanaOpção)</f>
         <v>44781</v>
@@ -3027,7 +3072,7 @@
         <v>44787</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -3036,7 +3081,7 @@
       <c r="G76" s="7"/>
       <c r="H76" s="8"/>
     </row>
-    <row r="77" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B77" s="10">
         <f t="array" aca="1" ref="B77:H77" ca="1">Dias+15+DATE(CalendárioAno6,CaléndárioMês6Opção,1)-WEEKDAY(DATE(CalendárioAno6,CaléndárioMês6Opção,1),DiaDaSemanaOpção)</f>
         <v>44788</v>
@@ -3066,7 +3111,7 @@
         <v>44794</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -3075,7 +3120,7 @@
       <c r="G78" s="7"/>
       <c r="H78" s="8"/>
     </row>
-    <row r="79" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B79" s="10">
         <f t="array" aca="1" ref="B79:H79" ca="1">Dias+22+DATE(CalendárioAno6,CaléndárioMês6Opção,1)-WEEKDAY(DATE(CalendárioAno6,CaléndárioMês6Opção,1),DiaDaSemanaOpção)</f>
         <v>44795</v>
@@ -3105,7 +3150,7 @@
         <v>44801</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -3114,7 +3159,7 @@
       <c r="G80" s="7"/>
       <c r="H80" s="8"/>
     </row>
-    <row r="81" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B81" s="10">
         <f t="array" aca="1" ref="B81:H81" ca="1">Dias+29+DATE(CalendárioAno6,CaléndárioMês6Opção,1)-WEEKDAY(DATE(CalendárioAno6,CaléndárioMês6Opção,1),DiaDaSemanaOpção)</f>
         <v>44802</v>
@@ -3144,7 +3189,7 @@
         <v>44808</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -3153,7 +3198,7 @@
       <c r="G82" s="7"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B83" s="10">
         <f t="array" aca="1" ref="B83:C83" ca="1">Dias+36+DATE(CalendárioAno6,CaléndárioMês6Opção,1)-WEEKDAY(DATE(CalendárioAno6,CaléndárioMês6Opção,1),DiaDaSemanaOpção)</f>
         <v>44809</v>
@@ -3162,40 +3207,40 @@
         <f ca="1"/>
         <v>44810</v>
       </c>
-      <c r="D83" s="36" t="s">
+      <c r="D83" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="37"/>
-    </row>
-    <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="36"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="39"/>
-    </row>
-    <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="34"/>
+      <c r="G84" s="34"/>
+      <c r="H84" s="34"/>
+    </row>
+    <row r="85" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A85" s="2"/>
       <c r="B85" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C85" s="35" t="str">
+      <c r="C85" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1),"mmmm")</f>
         <v>setembro</v>
       </c>
-      <c r="D85" s="35"/>
-      <c r="E85" s="35"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="4" t="str">
         <f t="shared" ref="B86:H86" ca="1" si="6">UPPER(TEXT(B87,"dddd"))</f>
@@ -3226,7 +3271,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B87" s="10">
         <f t="array" aca="1" ref="B87:H87" ca="1">Dias+1+DATE(CalendárioAno7,CaléndárioMês7Opção,1)-WEEKDAY(DATE(CalendárioAno7,CaléndárioMês7Opção,1),DiaDaSemanaOpção)</f>
         <v>44802</v>
@@ -3256,7 +3301,7 @@
         <v>44808</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -3265,7 +3310,7 @@
       <c r="G88" s="7"/>
       <c r="H88" s="8"/>
     </row>
-    <row r="89" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B89" s="10">
         <f t="array" aca="1" ref="B89:H89" ca="1">Dias+8+DATE(CalendárioAno7,CaléndárioMês7Opção,1)-WEEKDAY(DATE(CalendárioAno7,CaléndárioMês7Opção,1),DiaDaSemanaOpção)</f>
         <v>44809</v>
@@ -3295,7 +3340,7 @@
         <v>44815</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -3304,7 +3349,7 @@
       <c r="G90" s="7"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B91" s="10">
         <f t="array" aca="1" ref="B91:H91" ca="1">Dias+15+DATE(CalendárioAno7,CaléndárioMês7Opção,1)-WEEKDAY(DATE(CalendárioAno7,CaléndárioMês7Opção,1),DiaDaSemanaOpção)</f>
         <v>44816</v>
@@ -3334,7 +3379,7 @@
         <v>44822</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -3343,7 +3388,7 @@
       <c r="G92" s="7"/>
       <c r="H92" s="8"/>
     </row>
-    <row r="93" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B93" s="10">
         <f t="array" aca="1" ref="B93:H93" ca="1">Dias+22+DATE(CalendárioAno7,CaléndárioMês7Opção,1)-WEEKDAY(DATE(CalendárioAno7,CaléndárioMês7Opção,1),DiaDaSemanaOpção)</f>
         <v>44823</v>
@@ -3373,7 +3418,7 @@
         <v>44829</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -3382,7 +3427,7 @@
       <c r="G94" s="7"/>
       <c r="H94" s="8"/>
     </row>
-    <row r="95" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B95" s="10">
         <f t="array" aca="1" ref="B95:H95" ca="1">Dias+29+DATE(CalendárioAno7,CaléndárioMês7Opção,1)-WEEKDAY(DATE(CalendárioAno7,CaléndárioMês7Opção,1),DiaDaSemanaOpção)</f>
         <v>44830</v>
@@ -3412,7 +3457,7 @@
         <v>44836</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -3421,7 +3466,7 @@
       <c r="G96" s="7"/>
       <c r="H96" s="9"/>
     </row>
-    <row r="97" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B97" s="10">
         <f t="array" aca="1" ref="B97:C97" ca="1">Dias+36+DATE(CalendárioAno7,CaléndárioMês7Opção,1)-WEEKDAY(DATE(CalendárioAno7,CaléndárioMês7Opção,1),DiaDaSemanaOpção)</f>
         <v>44837</v>
@@ -3430,40 +3475,40 @@
         <f ca="1"/>
         <v>44838</v>
       </c>
-      <c r="D97" s="36" t="s">
+      <c r="D97" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="37"/>
-    </row>
-    <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="36"/>
+      <c r="F97" s="36"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="36"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
-    </row>
-    <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="34"/>
+    </row>
+    <row r="99" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A99" s="2"/>
       <c r="B99" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C99" s="35" t="str">
+      <c r="C99" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1),"mmmm")</f>
         <v>outubro</v>
       </c>
-      <c r="D99" s="35"/>
-      <c r="E99" s="35"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="4" t="str">
         <f t="shared" ref="B100:H100" ca="1" si="7">UPPER(TEXT(B101,"dddd"))</f>
@@ -3494,7 +3539,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B101" s="10">
         <f t="array" aca="1" ref="B101:H101" ca="1">Dias+1+DATE(CalendárioAno8,CaléndárioMês8Opção,1)-WEEKDAY(DATE(CalendárioAno8,CaléndárioMês8Opção,1),DiaDaSemanaOpção)</f>
         <v>44830</v>
@@ -3524,7 +3569,7 @@
         <v>44836</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -3533,7 +3578,7 @@
       <c r="G102" s="7"/>
       <c r="H102" s="8"/>
     </row>
-    <row r="103" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B103" s="10">
         <f t="array" aca="1" ref="B103:H103" ca="1">Dias+8+DATE(CalendárioAno8,CaléndárioMês8Opção,1)-WEEKDAY(DATE(CalendárioAno8,CaléndárioMês8Opção,1),DiaDaSemanaOpção)</f>
         <v>44837</v>
@@ -3563,7 +3608,7 @@
         <v>44843</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -3572,7 +3617,7 @@
       <c r="G104" s="7"/>
       <c r="H104" s="8"/>
     </row>
-    <row r="105" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B105" s="10">
         <f t="array" aca="1" ref="B105:H105" ca="1">Dias+15+DATE(CalendárioAno8,CaléndárioMês8Opção,1)-WEEKDAY(DATE(CalendárioAno8,CaléndárioMês8Opção,1),DiaDaSemanaOpção)</f>
         <v>44844</v>
@@ -3602,7 +3647,7 @@
         <v>44850</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -3611,7 +3656,7 @@
       <c r="G106" s="7"/>
       <c r="H106" s="8"/>
     </row>
-    <row r="107" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B107" s="10">
         <f t="array" aca="1" ref="B107:H107" ca="1">Dias+22+DATE(CalendárioAno8,CaléndárioMês8Opção,1)-WEEKDAY(DATE(CalendárioAno8,CaléndárioMês8Opção,1),DiaDaSemanaOpção)</f>
         <v>44851</v>
@@ -3641,7 +3686,7 @@
         <v>44857</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -3650,7 +3695,7 @@
       <c r="G108" s="7"/>
       <c r="H108" s="8"/>
     </row>
-    <row r="109" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B109" s="10">
         <f t="array" aca="1" ref="B109:H109" ca="1">Dias+29+DATE(CalendárioAno8,CaléndárioMês8Opção,1)-WEEKDAY(DATE(CalendárioAno8,CaléndárioMês8Opção,1),DiaDaSemanaOpção)</f>
         <v>44858</v>
@@ -3680,7 +3725,7 @@
         <v>44864</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -3689,7 +3734,7 @@
       <c r="G110" s="7"/>
       <c r="H110" s="9"/>
     </row>
-    <row r="111" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B111" s="10">
         <f t="array" aca="1" ref="B111:C111" ca="1">Dias+36+DATE(CalendárioAno8,CaléndárioMês8Opção,1)-WEEKDAY(DATE(CalendárioAno8,CaléndárioMês8Opção,1),DiaDaSemanaOpção)</f>
         <v>44865</v>
@@ -3698,40 +3743,40 @@
         <f ca="1"/>
         <v>44866</v>
       </c>
-      <c r="D111" s="36" t="s">
+      <c r="D111" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="37"/>
-      <c r="F111" s="37"/>
-      <c r="G111" s="37"/>
-      <c r="H111" s="37"/>
-    </row>
-    <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E111" s="36"/>
+      <c r="F111" s="36"/>
+      <c r="G111" s="36"/>
+      <c r="H111" s="36"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
-      <c r="F112" s="39"/>
-      <c r="G112" s="39"/>
-      <c r="H112" s="39"/>
-    </row>
-    <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D112" s="34"/>
+      <c r="E112" s="34"/>
+      <c r="F112" s="34"/>
+      <c r="G112" s="34"/>
+      <c r="H112" s="34"/>
+    </row>
+    <row r="113" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A113" s="2"/>
       <c r="B113" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C113" s="35" t="str">
+      <c r="C113" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1),"mmmm")</f>
         <v>novembro</v>
       </c>
-      <c r="D113" s="35"/>
-      <c r="E113" s="35"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="4" t="str">
         <f t="shared" ref="B114:H114" ca="1" si="8">UPPER(TEXT(B115,"dddd"))</f>
@@ -3762,7 +3807,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B115" s="10">
         <f t="array" aca="1" ref="B115:H115" ca="1">Dias+1+DATE(CalendárioAno9,CaléndárioMês9Opção,1)-WEEKDAY(DATE(CalendárioAno9,CaléndárioMês9Opção,1),DiaDaSemanaOpção)</f>
         <v>44865</v>
@@ -3792,7 +3837,7 @@
         <v>44871</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -3801,7 +3846,7 @@
       <c r="G116" s="7"/>
       <c r="H116" s="8"/>
     </row>
-    <row r="117" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B117" s="10">
         <f t="array" aca="1" ref="B117:H117" ca="1">Dias+8+DATE(CalendárioAno9,CaléndárioMês9Opção,1)-WEEKDAY(DATE(CalendárioAno9,CaléndárioMês9Opção,1),DiaDaSemanaOpção)</f>
         <v>44872</v>
@@ -3831,7 +3876,7 @@
         <v>44878</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
@@ -3840,7 +3885,7 @@
       <c r="G118" s="7"/>
       <c r="H118" s="8"/>
     </row>
-    <row r="119" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B119" s="10">
         <f t="array" aca="1" ref="B119:H119" ca="1">Dias+15+DATE(CalendárioAno9,CaléndárioMês9Opção,1)-WEEKDAY(DATE(CalendárioAno9,CaléndárioMês9Opção,1),DiaDaSemanaOpção)</f>
         <v>44879</v>
@@ -3870,7 +3915,7 @@
         <v>44885</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -3879,7 +3924,7 @@
       <c r="G120" s="7"/>
       <c r="H120" s="8"/>
     </row>
-    <row r="121" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B121" s="10">
         <f t="array" aca="1" ref="B121:H121" ca="1">Dias+22+DATE(CalendárioAno9,CaléndárioMês9Opção,1)-WEEKDAY(DATE(CalendárioAno9,CaléndárioMês9Opção,1),DiaDaSemanaOpção)</f>
         <v>44886</v>
@@ -3909,7 +3954,7 @@
         <v>44892</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
@@ -3918,7 +3963,7 @@
       <c r="G122" s="7"/>
       <c r="H122" s="8"/>
     </row>
-    <row r="123" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B123" s="10">
         <f t="array" aca="1" ref="B123:H123" ca="1">Dias+29+DATE(CalendárioAno9,CaléndárioMês9Opção,1)-WEEKDAY(DATE(CalendárioAno9,CaléndárioMês9Opção,1),DiaDaSemanaOpção)</f>
         <v>44893</v>
@@ -3948,7 +3993,7 @@
         <v>44899</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
@@ -3957,7 +4002,7 @@
       <c r="G124" s="7"/>
       <c r="H124" s="9"/>
     </row>
-    <row r="125" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B125" s="10">
         <f t="array" aca="1" ref="B125:C125" ca="1">Dias+36+DATE(CalendárioAno9,CaléndárioMês9Opção,1)-WEEKDAY(DATE(CalendárioAno9,CaléndárioMês9Opção,1),DiaDaSemanaOpção)</f>
         <v>44900</v>
@@ -3966,40 +4011,40 @@
         <f ca="1"/>
         <v>44901</v>
       </c>
-      <c r="D125" s="36" t="s">
+      <c r="D125" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="37"/>
-      <c r="H125" s="37"/>
-    </row>
-    <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E125" s="36"/>
+      <c r="F125" s="36"/>
+      <c r="G125" s="36"/>
+      <c r="H125" s="36"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="39"/>
-      <c r="F126" s="39"/>
-      <c r="G126" s="39"/>
-      <c r="H126" s="39"/>
-    </row>
-    <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D126" s="34"/>
+      <c r="E126" s="34"/>
+      <c r="F126" s="34"/>
+      <c r="G126" s="34"/>
+      <c r="H126" s="34"/>
+    </row>
+    <row r="127" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A127" s="2"/>
       <c r="B127" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C127" s="35" t="str">
+      <c r="C127" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1),"mmmm")</f>
         <v>dezembro</v>
       </c>
-      <c r="D127" s="35"/>
-      <c r="E127" s="35"/>
+      <c r="D127" s="37"/>
+      <c r="E127" s="37"/>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
       <c r="H127" s="2"/>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="4" t="str">
         <f ca="1">UPPER(TEXT(B129,"dddd"))</f>
@@ -4030,7 +4075,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="129" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B129" s="10">
         <f t="array" aca="1" ref="B129:H129" ca="1">Dias+1+DATE(CalendárioAno10,CaléndárioMês10Opção,1)-WEEKDAY(DATE(CalendárioAno10,CaléndárioMês10Opção,1),DiaDaSemanaOpção)</f>
         <v>44893</v>
@@ -4060,7 +4105,7 @@
         <v>44899</v>
       </c>
     </row>
-    <row r="130" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
@@ -4069,7 +4114,7 @@
       <c r="G130" s="7"/>
       <c r="H130" s="8"/>
     </row>
-    <row r="131" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B131" s="10">
         <f t="array" aca="1" ref="B131:H131" ca="1">Dias+8+DATE(CalendárioAno10,CaléndárioMês10Opção,1)-WEEKDAY(DATE(CalendárioAno10,CaléndárioMês10Opção,1),DiaDaSemanaOpção)</f>
         <v>44900</v>
@@ -4099,7 +4144,7 @@
         <v>44906</v>
       </c>
     </row>
-    <row r="132" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
@@ -4108,7 +4153,7 @@
       <c r="G132" s="7"/>
       <c r="H132" s="8"/>
     </row>
-    <row r="133" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B133" s="10">
         <f t="array" aca="1" ref="B133:H133" ca="1">Dias+15+DATE(CalendárioAno10,CaléndárioMês10Opção,1)-WEEKDAY(DATE(CalendárioAno10,CaléndárioMês10Opção,1),DiaDaSemanaOpção)</f>
         <v>44907</v>
@@ -4138,7 +4183,7 @@
         <v>44913</v>
       </c>
     </row>
-    <row r="134" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
@@ -4147,7 +4192,7 @@
       <c r="G134" s="7"/>
       <c r="H134" s="8"/>
     </row>
-    <row r="135" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B135" s="10">
         <f t="array" aca="1" ref="B135:H135" ca="1">Dias+22+DATE(CalendárioAno10,CaléndárioMês10Opção,1)-WEEKDAY(DATE(CalendárioAno10,CaléndárioMês10Opção,1),DiaDaSemanaOpção)</f>
         <v>44914</v>
@@ -4177,7 +4222,7 @@
         <v>44920</v>
       </c>
     </row>
-    <row r="136" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
@@ -4186,7 +4231,7 @@
       <c r="G136" s="7"/>
       <c r="H136" s="8"/>
     </row>
-    <row r="137" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B137" s="10">
         <f t="array" aca="1" ref="B137:H137" ca="1">Dias+29+DATE(CalendárioAno10,CaléndárioMês10Opção,1)-WEEKDAY(DATE(CalendárioAno10,CaléndárioMês10Opção,1),DiaDaSemanaOpção)</f>
         <v>44921</v>
@@ -4216,7 +4261,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="138" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
@@ -4225,7 +4270,7 @@
       <c r="G138" s="7"/>
       <c r="H138" s="9"/>
     </row>
-    <row r="139" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B139" s="10">
         <f t="array" aca="1" ref="B139:C139" ca="1">Dias+36+DATE(CalendárioAno10,CaléndárioMês10Opção,1)-WEEKDAY(DATE(CalendárioAno10,CaléndárioMês10Opção,1),DiaDaSemanaOpção)</f>
         <v>44928</v>
@@ -4234,39 +4279,39 @@
         <f ca="1"/>
         <v>44929</v>
       </c>
-      <c r="D139" s="36" t="s">
+      <c r="D139" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="37"/>
-      <c r="F139" s="37"/>
-      <c r="G139" s="37"/>
-      <c r="H139" s="37"/>
-    </row>
-    <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E139" s="36"/>
+      <c r="F139" s="36"/>
+      <c r="G139" s="36"/>
+      <c r="H139" s="36"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
-      <c r="D140" s="39"/>
-      <c r="E140" s="39"/>
-      <c r="F140" s="39"/>
-      <c r="G140" s="39"/>
-      <c r="H140" s="39"/>
-    </row>
-    <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D140" s="34"/>
+      <c r="E140" s="34"/>
+      <c r="F140" s="34"/>
+      <c r="G140" s="34"/>
+      <c r="H140" s="34"/>
+    </row>
+    <row r="141" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B141" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C141" s="35" t="str">
+      <c r="C141" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1),"mmmm")</f>
         <v>janeiro</v>
       </c>
-      <c r="D141" s="35"/>
-      <c r="E141" s="35"/>
+      <c r="D141" s="37"/>
+      <c r="E141" s="37"/>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
       <c r="H141" s="2"/>
     </row>
-    <row r="142" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B142" s="4" t="str">
         <f ca="1">UPPER(TEXT(B143,"dddd"))</f>
         <v>SEGUNDA-FEIRA</v>
@@ -4296,7 +4341,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="143" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B143" s="10">
         <f t="array" aca="1" ref="B143:H143" ca="1">Dias+1+DATE(CalendárioAno11,CaléndárioMês11Opção,1)-WEEKDAY(DATE(CalendárioAno11,CaléndárioMês11Opção,1),DiaDaSemanaOpção)</f>
         <v>44921</v>
@@ -4326,7 +4371,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="144" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
@@ -4335,7 +4380,7 @@
       <c r="G144" s="7"/>
       <c r="H144" s="8"/>
     </row>
-    <row r="145" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B145" s="10">
         <f t="array" aca="1" ref="B145:H145" ca="1">Dias+8+DATE(CalendárioAno11,CaléndárioMês11Opção,1)-WEEKDAY(DATE(CalendárioAno11,CaléndárioMês11Opção,1),DiaDaSemanaOpção)</f>
         <v>44928</v>
@@ -4365,7 +4410,7 @@
         <v>44934</v>
       </c>
     </row>
-    <row r="146" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
@@ -4374,7 +4419,7 @@
       <c r="G146" s="7"/>
       <c r="H146" s="8"/>
     </row>
-    <row r="147" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B147" s="10">
         <f t="array" aca="1" ref="B147:H147" ca="1">Dias+15+DATE(CalendárioAno11,CaléndárioMês11Opção,1)-WEEKDAY(DATE(CalendárioAno11,CaléndárioMês11Opção,1),DiaDaSemanaOpção)</f>
         <v>44935</v>
@@ -4404,7 +4449,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="148" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
@@ -4413,7 +4458,7 @@
       <c r="G148" s="7"/>
       <c r="H148" s="8"/>
     </row>
-    <row r="149" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B149" s="10">
         <f t="array" aca="1" ref="B149:H149" ca="1">Dias+22+DATE(CalendárioAno11,CaléndárioMês11Opção,1)-WEEKDAY(DATE(CalendárioAno11,CaléndárioMês11Opção,1),DiaDaSemanaOpção)</f>
         <v>44942</v>
@@ -4443,7 +4488,7 @@
         <v>44948</v>
       </c>
     </row>
-    <row r="150" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
@@ -4452,7 +4497,7 @@
       <c r="G150" s="7"/>
       <c r="H150" s="8"/>
     </row>
-    <row r="151" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B151" s="10">
         <f t="array" aca="1" ref="B151:H151" ca="1">Dias+29+DATE(CalendárioAno11,CaléndárioMês11Opção,1)-WEEKDAY(DATE(CalendárioAno11,CaléndárioMês11Opção,1),DiaDaSemanaOpção)</f>
         <v>44949</v>
@@ -4482,7 +4527,7 @@
         <v>44955</v>
       </c>
     </row>
-    <row r="152" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
@@ -4491,7 +4536,7 @@
       <c r="G152" s="7"/>
       <c r="H152" s="9"/>
     </row>
-    <row r="153" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B153" s="10">
         <f t="array" aca="1" ref="B153:C153" ca="1">Dias+36+DATE(CalendárioAno11,CaléndárioMês11Opção,1)-WEEKDAY(DATE(CalendárioAno11,CaléndárioMês11Opção,1),DiaDaSemanaOpção)</f>
         <v>44956</v>
@@ -4500,39 +4545,39 @@
         <f ca="1"/>
         <v>44957</v>
       </c>
-      <c r="D153" s="36" t="s">
+      <c r="D153" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="37"/>
-      <c r="F153" s="37"/>
-      <c r="G153" s="37"/>
-      <c r="H153" s="37"/>
-    </row>
-    <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E153" s="36"/>
+      <c r="F153" s="36"/>
+      <c r="G153" s="36"/>
+      <c r="H153" s="36"/>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
-      <c r="D154" s="39"/>
-      <c r="E154" s="39"/>
-      <c r="F154" s="39"/>
-      <c r="G154" s="39"/>
-      <c r="H154" s="39"/>
-    </row>
-    <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D154" s="34"/>
+      <c r="E154" s="34"/>
+      <c r="F154" s="34"/>
+      <c r="G154" s="34"/>
+      <c r="H154" s="34"/>
+    </row>
+    <row r="155" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B155" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C155" s="35" t="str">
+      <c r="C155" s="37" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1),"mmmm")</f>
         <v>fevereiro</v>
       </c>
-      <c r="D155" s="35"/>
-      <c r="E155" s="35"/>
+      <c r="D155" s="37"/>
+      <c r="E155" s="37"/>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
       <c r="H155" s="2"/>
     </row>
-    <row r="156" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B156" s="4" t="str">
         <f ca="1">UPPER(TEXT(B157,"dddd"))</f>
         <v>SEGUNDA-FEIRA</v>
@@ -4562,7 +4607,7 @@
         <v>DOMINGO</v>
       </c>
     </row>
-    <row r="157" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B157" s="10">
         <f t="array" aca="1" ref="B157:H157" ca="1">Dias+1+DATE(CalendárioAno12,CaléndárioMês12Opção,1)-WEEKDAY(DATE(CalendárioAno12,CaléndárioMês12Opção,1),DiaDaSemanaOpção)</f>
         <v>44956</v>
@@ -4592,7 +4637,7 @@
         <v>44962</v>
       </c>
     </row>
-    <row r="158" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
@@ -4601,7 +4646,7 @@
       <c r="G158" s="7"/>
       <c r="H158" s="8"/>
     </row>
-    <row r="159" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B159" s="10">
         <f t="array" aca="1" ref="B159:H159" ca="1">Dias+8+DATE(CalendárioAno12,CaléndárioMês12Opção,1)-WEEKDAY(DATE(CalendárioAno12,CaléndárioMês12Opção,1),DiaDaSemanaOpção)</f>
         <v>44963</v>
@@ -4631,7 +4676,7 @@
         <v>44969</v>
       </c>
     </row>
-    <row r="160" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -4640,7 +4685,7 @@
       <c r="G160" s="7"/>
       <c r="H160" s="8"/>
     </row>
-    <row r="161" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B161" s="10">
         <f t="array" aca="1" ref="B161:H161" ca="1">Dias+15+DATE(CalendárioAno12,CaléndárioMês12Opção,1)-WEEKDAY(DATE(CalendárioAno12,CaléndárioMês12Opção,1),DiaDaSemanaOpção)</f>
         <v>44970</v>
@@ -4670,7 +4715,7 @@
         <v>44976</v>
       </c>
     </row>
-    <row r="162" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
@@ -4679,7 +4724,7 @@
       <c r="G162" s="7"/>
       <c r="H162" s="8"/>
     </row>
-    <row r="163" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B163" s="10">
         <f t="array" aca="1" ref="B163:H163" ca="1">Dias+22+DATE(CalendárioAno12,CaléndárioMês12Opção,1)-WEEKDAY(DATE(CalendárioAno12,CaléndárioMês12Opção,1),DiaDaSemanaOpção)</f>
         <v>44977</v>
@@ -4709,7 +4754,7 @@
         <v>44983</v>
       </c>
     </row>
-    <row r="164" spans="2:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
@@ -4718,7 +4763,7 @@
       <c r="G164" s="7"/>
       <c r="H164" s="8"/>
     </row>
-    <row r="165" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B165" s="10">
         <f t="array" aca="1" ref="B165:H165" ca="1">Dias+29+DATE(CalendárioAno12,CaléndárioMês12Opção,1)-WEEKDAY(DATE(CalendárioAno12,CaléndárioMês12Opção,1),DiaDaSemanaOpção)</f>
         <v>44984</v>
@@ -4748,7 +4793,7 @@
         <v>44990</v>
       </c>
     </row>
-    <row r="166" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
@@ -4757,7 +4802,7 @@
       <c r="G166" s="7"/>
       <c r="H166" s="9"/>
     </row>
-    <row r="167" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:8" ht="21" x14ac:dyDescent="0.3">
       <c r="B167" s="10">
         <f t="array" aca="1" ref="B167:C167" ca="1">Dias+36+DATE(CalendárioAno12,CaléndárioMês12Opção,1)-WEEKDAY(DATE(CalendárioAno12,CaléndárioMês12Opção,1),DiaDaSemanaOpção)</f>
         <v>44991</v>
@@ -4766,25 +4811,45 @@
         <f ca="1"/>
         <v>44992</v>
       </c>
-      <c r="D167" s="36" t="s">
+      <c r="D167" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="37"/>
-      <c r="F167" s="37"/>
-      <c r="G167" s="37"/>
-      <c r="H167" s="37"/>
-    </row>
-    <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E167" s="36"/>
+      <c r="F167" s="36"/>
+      <c r="G167" s="36"/>
+      <c r="H167" s="36"/>
+    </row>
+    <row r="168" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
-      <c r="D168" s="39"/>
-      <c r="E168" s="39"/>
-      <c r="F168" s="39"/>
-      <c r="G168" s="39"/>
-      <c r="H168" s="39"/>
+      <c r="D168" s="34"/>
+      <c r="E168" s="34"/>
+      <c r="F168" s="34"/>
+      <c r="G168" s="34"/>
+      <c r="H168" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="D83:H83"/>
+    <mergeCell ref="D153:H153"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="D69:H69"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C99:E99"/>
     <mergeCell ref="D168:H168"/>
     <mergeCell ref="D139:H139"/>
     <mergeCell ref="D140:H140"/>
@@ -4801,26 +4866,6 @@
     <mergeCell ref="C127:E127"/>
     <mergeCell ref="C141:E141"/>
     <mergeCell ref="C155:E155"/>
-    <mergeCell ref="D153:H153"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="D70:H70"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="D83:H83"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">
@@ -4930,11 +4975,11 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4950,370 +4995,370 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="34">
+      <c r="C1" s="40"/>
+      <c r="D1" s="33">
         <v>25</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="21">
+      <c r="A3" s="20">
         <v>44635</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>44640</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="30" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="21">
+      <c r="A5" s="20">
         <v>44642</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>44647</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>44649</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="21">
         <v>44654</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="24" t="s">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
+      <c r="A9" s="20">
         <v>44656</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="21">
         <v>44661</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>44663</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="A12" s="21">
         <v>44668</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
+      <c r="A13" s="20">
         <v>44670</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="22">
+      <c r="A14" s="21">
         <v>44675</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
+      <c r="A15" s="20">
         <v>44677</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="22">
+      <c r="A16" s="21">
         <v>44682</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>44684</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
+      <c r="A18" s="21">
         <v>44689</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
+      <c r="A19" s="20">
         <v>44691</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="21">
         <v>44696</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
+      <c r="A21" s="20">
         <v>44698</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="22">
+      <c r="A22" s="21">
         <v>44703</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="21">
+      <c r="A23" s="20">
         <v>44705</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="27" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="22">
+      <c r="A24" s="21">
         <v>44710</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="27" t="s">
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="21">
+      <c r="A25" s="20">
         <v>44712</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="27" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="22">
+      <c r="A26" s="21">
         <v>44717</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="27" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="33">
+      <c r="A27" s="32">
         <v>44718</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="21">
+      <c r="A28" s="20">
         <v>44719</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="32">
+      <c r="A29" s="31">
         <v>44720</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="50"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="31">
+      <c r="A30" s="30">
         <v>44723</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5328,6 +5373,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426e97fa315356fffbdcd9876fe988c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14b8f0def80e6d70ce3def20c90759ae" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -5548,25 +5611,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B0EC2F5-DB17-4B75-9677-570CB7A949FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5583,22 +5646,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Alterações na comunicação com o banco
</commit_message>
<xml_diff>
--- a/Calendário TG.xlsx
+++ b/Calendário TG.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66792A3C-B7A1-4F32-BCEE-29977ED0DA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA043862-6208-44DA-922C-FD43A15E7330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="788" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="788" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendário" sheetId="14" r:id="rId1"/>
@@ -108,42 +108,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Autor</author>
-  </authors>
-  <commentList>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{6A331112-39C1-4782-A304-323775936560}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Carlos:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Tempo levado para extrair os dados da bateria no Firebase para iniciar treinamento</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
   <si>
     <t>Anotações:</t>
   </si>
@@ -429,12 +395,6 @@
     <t>Carlos</t>
   </si>
   <si>
-    <t>Tempo extração Firebase</t>
-  </si>
-  <si>
-    <t>Tempo de treinamento</t>
-  </si>
-  <si>
     <t>Treinamento / Teste</t>
   </si>
   <si>
@@ -442,27 +402,6 @@
   </si>
   <si>
     <t>Épocas</t>
-  </si>
-  <si>
-    <t>6m 12.5s</t>
-  </si>
-  <si>
-    <t>2m 33.8s</t>
-  </si>
-  <si>
-    <t>0.9333</t>
-  </si>
-  <si>
-    <t>array([[[62,  1],
-        [ 4,  8]],
-       [[56,  0],
-        [ 0, 19]],
-       [[58,  4],
-        [ 0, 13]],
-       [[60,  0],
-        [ 0, 15]],
-       [[59,  0],
-        [ 1, 15]]], dtype=int64)</t>
   </si>
 </sst>
 </file>
@@ -477,7 +416,7 @@
     <numFmt numFmtId="166" formatCode="dd"/>
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Trebuchet MS"/>
@@ -686,17 +625,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
+      <u/>
+      <sz val="11"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="49">
@@ -1309,7 +1242,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="9">
       <alignment horizontal="center"/>
@@ -1410,8 +1343,11 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1419,11 +1355,11 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1458,8 +1394,8 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1909,11 +1845,11 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2175,11 +2111,11 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
     </row>
     <row r="15" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A15" s="2"/>
@@ -2187,12 +2123,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C15" s="45" t="str">
+      <c r="C15" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1),"mmmm")</f>
         <v>abril</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="2"/>
@@ -2444,22 +2380,22 @@
         <f ca="1"/>
         <v>44684</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
     </row>
     <row r="29" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A29" s="2"/>
@@ -2467,12 +2403,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C29" s="45" t="str">
+      <c r="C29" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1),"mmmm")</f>
         <v>maio</v>
       </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="2"/>
@@ -2715,22 +2651,22 @@
         <f ca="1"/>
         <v>44712</v>
       </c>
-      <c r="D41" s="44" t="s">
+      <c r="D41" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
     </row>
     <row r="43" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A43" s="2"/>
@@ -2738,12 +2674,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C43" s="45" t="str">
+      <c r="C43" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1),"mmmm")</f>
         <v>junho</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="2"/>
@@ -2985,22 +2921,22 @@
         <f ca="1"/>
         <v>44747</v>
       </c>
-      <c r="D55" s="43" t="s">
+      <c r="D55" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
     </row>
     <row r="57" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A57" s="2"/>
@@ -3008,12 +2944,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C57" s="45" t="str">
+      <c r="C57" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1),"mmmm")</f>
         <v>julho</v>
       </c>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
+      <c r="D57" s="43"/>
+      <c r="E57" s="43"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="2"/>
@@ -3253,22 +3189,22 @@
         <f ca="1"/>
         <v>44775</v>
       </c>
-      <c r="D69" s="43" t="s">
+      <c r="D69" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="44"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="42"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
     </row>
     <row r="71" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A71" s="2"/>
@@ -3276,12 +3212,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C71" s="45" t="str">
+      <c r="C71" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1),"mmmm")</f>
         <v>agosto</v>
       </c>
-      <c r="D71" s="45"/>
-      <c r="E71" s="45"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="43"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="2"/>
@@ -3521,22 +3457,22 @@
         <f ca="1"/>
         <v>44810</v>
       </c>
-      <c r="D83" s="43" t="s">
+      <c r="D83" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="44"/>
+      <c r="E83" s="45"/>
+      <c r="F83" s="45"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="45"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
-      <c r="D84" s="42"/>
-      <c r="E84" s="42"/>
-      <c r="F84" s="42"/>
-      <c r="G84" s="42"/>
-      <c r="H84" s="42"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="47"/>
     </row>
     <row r="85" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A85" s="2"/>
@@ -3544,12 +3480,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C85" s="45" t="str">
+      <c r="C85" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1),"mmmm")</f>
         <v>setembro</v>
       </c>
-      <c r="D85" s="45"/>
-      <c r="E85" s="45"/>
+      <c r="D85" s="43"/>
+      <c r="E85" s="43"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="2"/>
@@ -3789,22 +3725,22 @@
         <f ca="1"/>
         <v>44838</v>
       </c>
-      <c r="D97" s="43" t="s">
+      <c r="D97" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="44"/>
-      <c r="F97" s="44"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="44"/>
+      <c r="E97" s="45"/>
+      <c r="F97" s="45"/>
+      <c r="G97" s="45"/>
+      <c r="H97" s="45"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
-      <c r="D98" s="42"/>
-      <c r="E98" s="42"/>
-      <c r="F98" s="42"/>
-      <c r="G98" s="42"/>
-      <c r="H98" s="42"/>
+      <c r="D98" s="47"/>
+      <c r="E98" s="47"/>
+      <c r="F98" s="47"/>
+      <c r="G98" s="47"/>
+      <c r="H98" s="47"/>
     </row>
     <row r="99" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A99" s="2"/>
@@ -3812,12 +3748,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C99" s="45" t="str">
+      <c r="C99" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1),"mmmm")</f>
         <v>outubro</v>
       </c>
-      <c r="D99" s="45"/>
-      <c r="E99" s="45"/>
+      <c r="D99" s="43"/>
+      <c r="E99" s="43"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="2"/>
@@ -4057,22 +3993,22 @@
         <f ca="1"/>
         <v>44866</v>
       </c>
-      <c r="D111" s="43" t="s">
+      <c r="D111" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="44"/>
-      <c r="F111" s="44"/>
-      <c r="G111" s="44"/>
-      <c r="H111" s="44"/>
+      <c r="E111" s="45"/>
+      <c r="F111" s="45"/>
+      <c r="G111" s="45"/>
+      <c r="H111" s="45"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
-      <c r="D112" s="42"/>
-      <c r="E112" s="42"/>
-      <c r="F112" s="42"/>
-      <c r="G112" s="42"/>
-      <c r="H112" s="42"/>
+      <c r="D112" s="47"/>
+      <c r="E112" s="47"/>
+      <c r="F112" s="47"/>
+      <c r="G112" s="47"/>
+      <c r="H112" s="47"/>
     </row>
     <row r="113" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A113" s="2"/>
@@ -4080,12 +4016,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C113" s="45" t="str">
+      <c r="C113" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1),"mmmm")</f>
         <v>novembro</v>
       </c>
-      <c r="D113" s="45"/>
-      <c r="E113" s="45"/>
+      <c r="D113" s="43"/>
+      <c r="E113" s="43"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
       <c r="H113" s="2"/>
@@ -4325,22 +4261,22 @@
         <f ca="1"/>
         <v>44901</v>
       </c>
-      <c r="D125" s="43" t="s">
+      <c r="D125" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="44"/>
-      <c r="F125" s="44"/>
-      <c r="G125" s="44"/>
-      <c r="H125" s="44"/>
+      <c r="E125" s="45"/>
+      <c r="F125" s="45"/>
+      <c r="G125" s="45"/>
+      <c r="H125" s="45"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
-      <c r="D126" s="42"/>
-      <c r="E126" s="42"/>
-      <c r="F126" s="42"/>
-      <c r="G126" s="42"/>
-      <c r="H126" s="42"/>
+      <c r="D126" s="47"/>
+      <c r="E126" s="47"/>
+      <c r="F126" s="47"/>
+      <c r="G126" s="47"/>
+      <c r="H126" s="47"/>
     </row>
     <row r="127" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A127" s="2"/>
@@ -4348,12 +4284,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C127" s="45" t="str">
+      <c r="C127" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1),"mmmm")</f>
         <v>dezembro</v>
       </c>
-      <c r="D127" s="45"/>
-      <c r="E127" s="45"/>
+      <c r="D127" s="43"/>
+      <c r="E127" s="43"/>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
       <c r="H127" s="2"/>
@@ -4593,34 +4529,34 @@
         <f ca="1"/>
         <v>44929</v>
       </c>
-      <c r="D139" s="43" t="s">
+      <c r="D139" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="44"/>
-      <c r="F139" s="44"/>
-      <c r="G139" s="44"/>
-      <c r="H139" s="44"/>
+      <c r="E139" s="45"/>
+      <c r="F139" s="45"/>
+      <c r="G139" s="45"/>
+      <c r="H139" s="45"/>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
-      <c r="D140" s="42"/>
-      <c r="E140" s="42"/>
-      <c r="F140" s="42"/>
-      <c r="G140" s="42"/>
-      <c r="H140" s="42"/>
+      <c r="D140" s="47"/>
+      <c r="E140" s="47"/>
+      <c r="F140" s="47"/>
+      <c r="G140" s="47"/>
+      <c r="H140" s="47"/>
     </row>
     <row r="141" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B141" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C141" s="45" t="str">
+      <c r="C141" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1),"mmmm")</f>
         <v>janeiro</v>
       </c>
-      <c r="D141" s="45"/>
-      <c r="E141" s="45"/>
+      <c r="D141" s="43"/>
+      <c r="E141" s="43"/>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
       <c r="H141" s="2"/>
@@ -4859,34 +4795,34 @@
         <f ca="1"/>
         <v>44957</v>
       </c>
-      <c r="D153" s="43" t="s">
+      <c r="D153" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="44"/>
-      <c r="F153" s="44"/>
-      <c r="G153" s="44"/>
-      <c r="H153" s="44"/>
+      <c r="E153" s="45"/>
+      <c r="F153" s="45"/>
+      <c r="G153" s="45"/>
+      <c r="H153" s="45"/>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
-      <c r="D154" s="42"/>
-      <c r="E154" s="42"/>
-      <c r="F154" s="42"/>
-      <c r="G154" s="42"/>
-      <c r="H154" s="42"/>
+      <c r="D154" s="47"/>
+      <c r="E154" s="47"/>
+      <c r="F154" s="47"/>
+      <c r="G154" s="47"/>
+      <c r="H154" s="47"/>
     </row>
     <row r="155" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B155" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C155" s="45" t="str">
+      <c r="C155" s="43" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1),"mmmm")</f>
         <v>fevereiro</v>
       </c>
-      <c r="D155" s="45"/>
-      <c r="E155" s="45"/>
+      <c r="D155" s="43"/>
+      <c r="E155" s="43"/>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
       <c r="H155" s="2"/>
@@ -5125,45 +5061,25 @@
         <f ca="1"/>
         <v>44992</v>
       </c>
-      <c r="D167" s="43" t="s">
+      <c r="D167" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="44"/>
-      <c r="F167" s="44"/>
-      <c r="G167" s="44"/>
-      <c r="H167" s="44"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="45"/>
+      <c r="G167" s="45"/>
+      <c r="H167" s="45"/>
     </row>
     <row r="168" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
-      <c r="D168" s="42"/>
-      <c r="E168" s="42"/>
-      <c r="F168" s="42"/>
-      <c r="G168" s="42"/>
-      <c r="H168" s="42"/>
+      <c r="D168" s="47"/>
+      <c r="E168" s="47"/>
+      <c r="F168" s="47"/>
+      <c r="G168" s="47"/>
+      <c r="H168" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="D83:H83"/>
-    <mergeCell ref="D153:H153"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="D70:H70"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C99:E99"/>
     <mergeCell ref="D168:H168"/>
     <mergeCell ref="D139:H139"/>
     <mergeCell ref="D140:H140"/>
@@ -5180,6 +5096,26 @@
     <mergeCell ref="C127:E127"/>
     <mergeCell ref="C141:E141"/>
     <mergeCell ref="C155:E155"/>
+    <mergeCell ref="D153:H153"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="D69:H69"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="D83:H83"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">
@@ -5312,10 +5248,10 @@
       <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="48"/>
+      <c r="C1" s="49"/>
       <c r="D1" s="33">
         <v>25</v>
       </c>
@@ -5628,14 +5564,14 @@
       <c r="A27" s="32">
         <v>44718</v>
       </c>
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
@@ -5652,27 +5588,27 @@
       <c r="A29" s="31">
         <v>44720</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="58"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="30">
         <v>44723</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5687,17 +5623,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFCB1CA-A9A5-4662-9F24-9BBCC5CF0095}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFCB1CA-A9A5-4662-9F24-9BBCC5CF0095}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AY11"/>
+  <dimension ref="A1:AY9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5925,7 +5861,7 @@
       <c r="B3" s="40">
         <v>44674</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
@@ -6091,10 +6027,10 @@
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -6148,10 +6084,10 @@
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="38">
-        <v>1000</v>
+        <v>88</v>
+      </c>
+      <c r="B7" s="59">
+        <v>500</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
@@ -6207,9 +6143,7 @@
       <c r="A8" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="38" t="s">
-        <v>93</v>
-      </c>
+      <c r="B8" s="38"/>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
@@ -6260,13 +6194,11 @@
       <c r="AX8" s="38"/>
       <c r="AY8" s="38"/>
     </row>
-    <row r="9" spans="1:51" ht="231" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="58" t="s">
-        <v>94</v>
-      </c>
+      <c r="B9" s="42"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -6317,147 +6249,14 @@
       <c r="AX9" s="38"/>
       <c r="AY9" s="38"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="38"/>
-      <c r="AD10" s="38"/>
-      <c r="AE10" s="38"/>
-      <c r="AF10" s="38"/>
-      <c r="AG10" s="38"/>
-      <c r="AH10" s="38"/>
-      <c r="AI10" s="38"/>
-      <c r="AJ10" s="38"/>
-      <c r="AK10" s="38"/>
-      <c r="AL10" s="38"/>
-      <c r="AM10" s="38"/>
-      <c r="AN10" s="38"/>
-      <c r="AO10" s="38"/>
-      <c r="AP10" s="38"/>
-      <c r="AQ10" s="38"/>
-      <c r="AR10" s="38"/>
-      <c r="AS10" s="38"/>
-      <c r="AT10" s="38"/>
-      <c r="AU10" s="38"/>
-      <c r="AV10" s="38"/>
-      <c r="AW10" s="38"/>
-      <c r="AX10" s="38"/>
-      <c r="AY10" s="38"/>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="38"/>
-      <c r="AJ11" s="38"/>
-      <c r="AK11" s="38"/>
-      <c r="AL11" s="38"/>
-      <c r="AM11" s="38"/>
-      <c r="AN11" s="38"/>
-      <c r="AO11" s="38"/>
-      <c r="AP11" s="38"/>
-      <c r="AQ11" s="38"/>
-      <c r="AR11" s="38"/>
-      <c r="AS11" s="38"/>
-      <c r="AT11" s="38"/>
-      <c r="AU11" s="38"/>
-      <c r="AV11" s="38"/>
-      <c r="AW11" s="38"/>
-      <c r="AX11" s="38"/>
-      <c r="AY11" s="38"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="27" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426e97fa315356fffbdcd9876fe988c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14b8f0def80e6d70ce3def20c90759ae" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -6678,25 +6477,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B0EC2F5-DB17-4B75-9677-570CB7A949FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6713,4 +6512,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Trabalhos relacionados e Calendário TG
Atualização da tabela de trabalhos relacionados e atualização das últimas reuniões TG
</commit_message>
<xml_diff>
--- a/Calendário TG.xlsx
+++ b/Calendário TG.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA043862-6208-44DA-922C-FD43A15E7330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A6959B-3779-407C-8974-CAD85FB1B911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="788" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendário" sheetId="14" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Anotações:</t>
   </si>
@@ -402,6 +402,24 @@
   </si>
   <si>
     <t>Épocas</t>
+  </si>
+  <si>
+    <t>&gt; Finalização de código Python para captura e treinamento
+&gt; Finalização de leitura de novos trabalhos relacionados</t>
+  </si>
+  <si>
+    <t>&gt; Leitura de trabalhos relacionados
+&gt; Primeiras baterias de teste realizadas</t>
+  </si>
+  <si>
+    <t>Próxima semana: 
+&gt; Finalização de leitura de novos trabalhos relacionados</t>
+  </si>
+  <si>
+    <t>Próxima semana: 
+&gt; Atualizar documentação em referencial teórico
+&gt; Atualizar documentação em trabalhos relacionados
+&gt; Continuar Coletas e Baterias de Teste</t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1364,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1355,11 +1376,11 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1393,9 +1414,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1826,8 +1844,8 @@
   </sheetPr>
   <dimension ref="A1:I168"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1845,11 +1863,11 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2100,22 +2118,22 @@
         <f ca="1"/>
         <v>44656</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A15" s="2"/>
@@ -2123,12 +2141,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C15" s="43" t="str">
+      <c r="C15" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1),"mmmm")</f>
         <v>abril</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="2"/>
@@ -2282,15 +2300,19 @@
         <v>44668</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="33.75" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="28"/>
+      <c r="H22" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B23" s="10">
@@ -2322,15 +2344,19 @@
         <v>44675</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="28"/>
+      <c r="H24" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
@@ -2380,22 +2406,22 @@
         <f ca="1"/>
         <v>44684</v>
       </c>
-      <c r="D27" s="45" t="s">
+      <c r="D27" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
     </row>
     <row r="29" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A29" s="2"/>
@@ -2403,12 +2429,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C29" s="43" t="str">
+      <c r="C29" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1),"mmmm")</f>
         <v>maio</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="2"/>
@@ -2651,22 +2677,22 @@
         <f ca="1"/>
         <v>44712</v>
       </c>
-      <c r="D41" s="45" t="s">
+      <c r="D41" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
     </row>
     <row r="43" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A43" s="2"/>
@@ -2674,12 +2700,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C43" s="43" t="str">
+      <c r="C43" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1),"mmmm")</f>
         <v>junho</v>
       </c>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="2"/>
@@ -2921,22 +2947,22 @@
         <f ca="1"/>
         <v>44747</v>
       </c>
-      <c r="D55" s="44" t="s">
+      <c r="D55" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
     </row>
     <row r="57" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A57" s="2"/>
@@ -2944,12 +2970,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C57" s="43" t="str">
+      <c r="C57" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1),"mmmm")</f>
         <v>julho</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="2"/>
@@ -3189,22 +3215,22 @@
         <f ca="1"/>
         <v>44775</v>
       </c>
-      <c r="D69" s="44" t="s">
+      <c r="D69" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="45"/>
-      <c r="H69" s="45"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="44"/>
     </row>
     <row r="71" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A71" s="2"/>
@@ -3212,12 +3238,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C71" s="43" t="str">
+      <c r="C71" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1),"mmmm")</f>
         <v>agosto</v>
       </c>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="2"/>
@@ -3457,22 +3483,22 @@
         <f ca="1"/>
         <v>44810</v>
       </c>
-      <c r="D83" s="44" t="s">
+      <c r="D83" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="45"/>
-      <c r="F83" s="45"/>
-      <c r="G83" s="45"/>
-      <c r="H83" s="45"/>
+      <c r="E83" s="46"/>
+      <c r="F83" s="46"/>
+      <c r="G83" s="46"/>
+      <c r="H83" s="46"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="47"/>
-      <c r="H84" s="47"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
     </row>
     <row r="85" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A85" s="2"/>
@@ -3480,12 +3506,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C85" s="43" t="str">
+      <c r="C85" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1),"mmmm")</f>
         <v>setembro</v>
       </c>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="2"/>
@@ -3725,22 +3751,22 @@
         <f ca="1"/>
         <v>44838</v>
       </c>
-      <c r="D97" s="44" t="s">
+      <c r="D97" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
+      <c r="E97" s="46"/>
+      <c r="F97" s="46"/>
+      <c r="G97" s="46"/>
+      <c r="H97" s="46"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
-      <c r="D98" s="47"/>
-      <c r="E98" s="47"/>
-      <c r="F98" s="47"/>
-      <c r="G98" s="47"/>
-      <c r="H98" s="47"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
     </row>
     <row r="99" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A99" s="2"/>
@@ -3748,12 +3774,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C99" s="43" t="str">
+      <c r="C99" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1),"mmmm")</f>
         <v>outubro</v>
       </c>
-      <c r="D99" s="43"/>
-      <c r="E99" s="43"/>
+      <c r="D99" s="47"/>
+      <c r="E99" s="47"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="2"/>
@@ -3993,22 +4019,22 @@
         <f ca="1"/>
         <v>44866</v>
       </c>
-      <c r="D111" s="44" t="s">
+      <c r="D111" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="45"/>
-      <c r="F111" s="45"/>
-      <c r="G111" s="45"/>
-      <c r="H111" s="45"/>
+      <c r="E111" s="46"/>
+      <c r="F111" s="46"/>
+      <c r="G111" s="46"/>
+      <c r="H111" s="46"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
-      <c r="G112" s="47"/>
-      <c r="H112" s="47"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
     </row>
     <row r="113" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A113" s="2"/>
@@ -4016,12 +4042,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C113" s="43" t="str">
+      <c r="C113" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1),"mmmm")</f>
         <v>novembro</v>
       </c>
-      <c r="D113" s="43"/>
-      <c r="E113" s="43"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
       <c r="H113" s="2"/>
@@ -4261,22 +4287,22 @@
         <f ca="1"/>
         <v>44901</v>
       </c>
-      <c r="D125" s="44" t="s">
+      <c r="D125" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="45"/>
-      <c r="F125" s="45"/>
-      <c r="G125" s="45"/>
-      <c r="H125" s="45"/>
+      <c r="E125" s="46"/>
+      <c r="F125" s="46"/>
+      <c r="G125" s="46"/>
+      <c r="H125" s="46"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
-      <c r="D126" s="47"/>
-      <c r="E126" s="47"/>
-      <c r="F126" s="47"/>
-      <c r="G126" s="47"/>
-      <c r="H126" s="47"/>
+      <c r="D126" s="44"/>
+      <c r="E126" s="44"/>
+      <c r="F126" s="44"/>
+      <c r="G126" s="44"/>
+      <c r="H126" s="44"/>
     </row>
     <row r="127" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A127" s="2"/>
@@ -4284,12 +4310,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C127" s="43" t="str">
+      <c r="C127" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1),"mmmm")</f>
         <v>dezembro</v>
       </c>
-      <c r="D127" s="43"/>
-      <c r="E127" s="43"/>
+      <c r="D127" s="47"/>
+      <c r="E127" s="47"/>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
       <c r="H127" s="2"/>
@@ -4529,34 +4555,34 @@
         <f ca="1"/>
         <v>44929</v>
       </c>
-      <c r="D139" s="44" t="s">
+      <c r="D139" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="45"/>
-      <c r="F139" s="45"/>
-      <c r="G139" s="45"/>
-      <c r="H139" s="45"/>
+      <c r="E139" s="46"/>
+      <c r="F139" s="46"/>
+      <c r="G139" s="46"/>
+      <c r="H139" s="46"/>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
-      <c r="D140" s="47"/>
-      <c r="E140" s="47"/>
-      <c r="F140" s="47"/>
-      <c r="G140" s="47"/>
-      <c r="H140" s="47"/>
+      <c r="D140" s="44"/>
+      <c r="E140" s="44"/>
+      <c r="F140" s="44"/>
+      <c r="G140" s="44"/>
+      <c r="H140" s="44"/>
     </row>
     <row r="141" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B141" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C141" s="43" t="str">
+      <c r="C141" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1),"mmmm")</f>
         <v>janeiro</v>
       </c>
-      <c r="D141" s="43"/>
-      <c r="E141" s="43"/>
+      <c r="D141" s="47"/>
+      <c r="E141" s="47"/>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
       <c r="H141" s="2"/>
@@ -4795,34 +4821,34 @@
         <f ca="1"/>
         <v>44957</v>
       </c>
-      <c r="D153" s="44" t="s">
+      <c r="D153" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="45"/>
-      <c r="F153" s="45"/>
-      <c r="G153" s="45"/>
-      <c r="H153" s="45"/>
+      <c r="E153" s="46"/>
+      <c r="F153" s="46"/>
+      <c r="G153" s="46"/>
+      <c r="H153" s="46"/>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
-      <c r="D154" s="47"/>
-      <c r="E154" s="47"/>
-      <c r="F154" s="47"/>
-      <c r="G154" s="47"/>
-      <c r="H154" s="47"/>
+      <c r="D154" s="44"/>
+      <c r="E154" s="44"/>
+      <c r="F154" s="44"/>
+      <c r="G154" s="44"/>
+      <c r="H154" s="44"/>
     </row>
     <row r="155" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B155" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C155" s="43" t="str">
+      <c r="C155" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1),"mmmm")</f>
         <v>fevereiro</v>
       </c>
-      <c r="D155" s="43"/>
-      <c r="E155" s="43"/>
+      <c r="D155" s="47"/>
+      <c r="E155" s="47"/>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
       <c r="H155" s="2"/>
@@ -5061,25 +5087,45 @@
         <f ca="1"/>
         <v>44992</v>
       </c>
-      <c r="D167" s="44" t="s">
+      <c r="D167" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="45"/>
-      <c r="F167" s="45"/>
-      <c r="G167" s="45"/>
-      <c r="H167" s="45"/>
+      <c r="E167" s="46"/>
+      <c r="F167" s="46"/>
+      <c r="G167" s="46"/>
+      <c r="H167" s="46"/>
     </row>
     <row r="168" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
-      <c r="D168" s="47"/>
-      <c r="E168" s="47"/>
-      <c r="F168" s="47"/>
-      <c r="G168" s="47"/>
-      <c r="H168" s="47"/>
+      <c r="D168" s="44"/>
+      <c r="E168" s="44"/>
+      <c r="F168" s="44"/>
+      <c r="G168" s="44"/>
+      <c r="H168" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="D83:H83"/>
+    <mergeCell ref="D153:H153"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="D69:H69"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C99:E99"/>
     <mergeCell ref="D168:H168"/>
     <mergeCell ref="D139:H139"/>
     <mergeCell ref="D140:H140"/>
@@ -5096,26 +5142,6 @@
     <mergeCell ref="C127:E127"/>
     <mergeCell ref="C141:E141"/>
     <mergeCell ref="C155:E155"/>
-    <mergeCell ref="D153:H153"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="D70:H70"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="D83:H83"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">
@@ -5248,10 +5274,10 @@
       <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="49"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="33">
         <v>25</v>
       </c>
@@ -5564,14 +5590,14 @@
       <c r="A27" s="32">
         <v>44718</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="56"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
@@ -5588,27 +5614,27 @@
       <c r="A29" s="31">
         <v>44720</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="30">
         <v>44723</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5629,11 +5655,11 @@
   </sheetPr>
   <dimension ref="A1:AY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6086,7 +6112,7 @@
       <c r="A7" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B7" s="43">
         <v>500</v>
       </c>
       <c r="C7" s="38"/>
@@ -6257,6 +6283,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426e97fa315356fffbdcd9876fe988c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14b8f0def80e6d70ce3def20c90759ae" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -6477,25 +6521,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B0EC2F5-DB17-4B75-9677-570CB7A949FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6512,22 +6556,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update baterias de teste
Realizada a bateria 2 e testes com as baterias 1 e 2
</commit_message>
<xml_diff>
--- a/Calendário TG.xlsx
+++ b/Calendário TG.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E891BC7-DBC0-474C-B191-08F52F938509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2695848-2B51-449A-9DAA-F7BEE4E4041F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="788" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Anotações:</t>
   </si>
@@ -274,96 +274,6 @@
   </si>
   <si>
     <t>BATERIA 20</t>
-  </si>
-  <si>
-    <t>BATERIA 21</t>
-  </si>
-  <si>
-    <t>BATERIA 22</t>
-  </si>
-  <si>
-    <t>BATERIA 23</t>
-  </si>
-  <si>
-    <t>BATERIA 24</t>
-  </si>
-  <si>
-    <t>BATERIA 25</t>
-  </si>
-  <si>
-    <t>BATERIA 26</t>
-  </si>
-  <si>
-    <t>BATERIA 27</t>
-  </si>
-  <si>
-    <t>BATERIA 28</t>
-  </si>
-  <si>
-    <t>BATERIA 29</t>
-  </si>
-  <si>
-    <t>BATERIA 30</t>
-  </si>
-  <si>
-    <t>BATERIA 31</t>
-  </si>
-  <si>
-    <t>BATERIA 32</t>
-  </si>
-  <si>
-    <t>BATERIA 33</t>
-  </si>
-  <si>
-    <t>BATERIA 34</t>
-  </si>
-  <si>
-    <t>BATERIA 35</t>
-  </si>
-  <si>
-    <t>BATERIA 36</t>
-  </si>
-  <si>
-    <t>BATERIA 37</t>
-  </si>
-  <si>
-    <t>BATERIA 38</t>
-  </si>
-  <si>
-    <t>BATERIA 39</t>
-  </si>
-  <si>
-    <t>BATERIA 40</t>
-  </si>
-  <si>
-    <t>BATERIA 41</t>
-  </si>
-  <si>
-    <t>BATERIA 42</t>
-  </si>
-  <si>
-    <t>BATERIA 43</t>
-  </si>
-  <si>
-    <t>BATERIA 44</t>
-  </si>
-  <si>
-    <t>BATERIA 45</t>
-  </si>
-  <si>
-    <t>BATERIA 46</t>
-  </si>
-  <si>
-    <t>BATERIA 47</t>
-  </si>
-  <si>
-    <t>BATERIA 48</t>
-  </si>
-  <si>
-    <t>BATERIA 49</t>
-  </si>
-  <si>
-    <t>BATERIA 50</t>
   </si>
   <si>
     <t>Data</t>
@@ -435,6 +345,36 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>array([[[60,  0],
+        [ 0, 15]],
+       [[60,  0],
+        [ 0, 15]],
+       [[60,  0],
+        [ 0, 15]],
+       [[60,  0],
+        [ 0, 15]],
+       [[60,  0],
+        [ 0, 15]]], dtype=int64)</t>
+  </si>
+  <si>
+    <t>BATERIAS 1 e 2</t>
+  </si>
+  <si>
+    <t>array([[[120,   0],
+        [ 30,   0]],
+       [[121,   0],
+        [ 29,   0]],
+       [[  0, 117],
+        [  0,  33]],
+       [[123,   0],
+        [ 27,   0]],
+       [[119,   0],
+        [ 31,   0]]], dtype=int64)</t>
+  </si>
+  <si>
+    <t>0.22</t>
   </si>
 </sst>
 </file>
@@ -449,7 +389,7 @@
     <numFmt numFmtId="166" formatCode="dd"/>
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Trebuchet MS"/>
@@ -660,6 +600,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1275,7 +1223,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="9">
       <alignment horizontal="center"/>
@@ -1382,8 +1330,8 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1391,11 +1339,11 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1429,6 +1377,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="48" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1878,11 +1829,11 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -2133,22 +2084,22 @@
         <f ca="1"/>
         <v>44656</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A15" s="2"/>
@@ -2156,12 +2107,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C15" s="44" t="str">
+      <c r="C15" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno1,CaléndárioMês1Opção+1,1),"mmmm")</f>
         <v>abril</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="2"/>
@@ -2279,10 +2230,10 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="34" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="I20" s="28" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.3">
@@ -2323,10 +2274,10 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="34" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.3">
@@ -2367,10 +2318,10 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="34" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="I24" s="28" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.3">
@@ -2432,11 +2383,11 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
     </row>
     <row r="29" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A29" s="2"/>
@@ -2444,12 +2395,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C29" s="44" t="str">
+      <c r="C29" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno2,CaléndárioMês2Opção+1,1),"mmmm")</f>
         <v>maio</v>
       </c>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="2"/>
@@ -2703,11 +2654,11 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
     </row>
     <row r="43" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A43" s="2"/>
@@ -2715,12 +2666,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C43" s="44" t="str">
+      <c r="C43" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno3,CaléndárioMês3Opção+1,1),"mmmm")</f>
         <v>junho</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="2"/>
@@ -2973,11 +2924,11 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
     </row>
     <row r="57" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A57" s="2"/>
@@ -2985,12 +2936,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C57" s="44" t="str">
+      <c r="C57" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno4,CaléndárioMês4Opção+1,1),"mmmm")</f>
         <v>julho</v>
       </c>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="2"/>
@@ -3241,11 +3192,11 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="44"/>
     </row>
     <row r="71" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A71" s="2"/>
@@ -3253,12 +3204,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C71" s="44" t="str">
+      <c r="C71" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno5,CaléndárioMês5Opção+1,1),"mmmm")</f>
         <v>agosto</v>
       </c>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="2"/>
@@ -3509,11 +3460,11 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="48"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
     </row>
     <row r="85" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A85" s="2"/>
@@ -3521,12 +3472,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C85" s="44" t="str">
+      <c r="C85" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno6,CaléndárioMês6Opção+1,1),"mmmm")</f>
         <v>setembro</v>
       </c>
-      <c r="D85" s="44"/>
-      <c r="E85" s="44"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="2"/>
@@ -3777,11 +3728,11 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
-      <c r="D98" s="48"/>
-      <c r="E98" s="48"/>
-      <c r="F98" s="48"/>
-      <c r="G98" s="48"/>
-      <c r="H98" s="48"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
     </row>
     <row r="99" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A99" s="2"/>
@@ -3789,12 +3740,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C99" s="44" t="str">
+      <c r="C99" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno7,CaléndárioMês7Opção+1,1),"mmmm")</f>
         <v>outubro</v>
       </c>
-      <c r="D99" s="44"/>
-      <c r="E99" s="44"/>
+      <c r="D99" s="47"/>
+      <c r="E99" s="47"/>
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
       <c r="H99" s="2"/>
@@ -4045,11 +3996,11 @@
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
-      <c r="D112" s="48"/>
-      <c r="E112" s="48"/>
-      <c r="F112" s="48"/>
-      <c r="G112" s="48"/>
-      <c r="H112" s="48"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
     </row>
     <row r="113" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A113" s="2"/>
@@ -4057,12 +4008,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C113" s="44" t="str">
+      <c r="C113" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno8,CaléndárioMês8Opção+1,1),"mmmm")</f>
         <v>novembro</v>
       </c>
-      <c r="D113" s="44"/>
-      <c r="E113" s="44"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
       <c r="H113" s="2"/>
@@ -4313,11 +4264,11 @@
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
-      <c r="D126" s="48"/>
-      <c r="E126" s="48"/>
-      <c r="F126" s="48"/>
-      <c r="G126" s="48"/>
-      <c r="H126" s="48"/>
+      <c r="D126" s="44"/>
+      <c r="E126" s="44"/>
+      <c r="F126" s="44"/>
+      <c r="G126" s="44"/>
+      <c r="H126" s="44"/>
     </row>
     <row r="127" spans="1:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A127" s="2"/>
@@ -4325,12 +4276,12 @@
         <f ca="1">YEAR(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1))</f>
         <v>2022</v>
       </c>
-      <c r="C127" s="44" t="str">
+      <c r="C127" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno9,CaléndárioMês9Opção+1,1),"mmmm")</f>
         <v>dezembro</v>
       </c>
-      <c r="D127" s="44"/>
-      <c r="E127" s="44"/>
+      <c r="D127" s="47"/>
+      <c r="E127" s="47"/>
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
       <c r="H127" s="2"/>
@@ -4581,23 +4532,23 @@
     <row r="140" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
-      <c r="D140" s="48"/>
-      <c r="E140" s="48"/>
-      <c r="F140" s="48"/>
-      <c r="G140" s="48"/>
-      <c r="H140" s="48"/>
+      <c r="D140" s="44"/>
+      <c r="E140" s="44"/>
+      <c r="F140" s="44"/>
+      <c r="G140" s="44"/>
+      <c r="H140" s="44"/>
     </row>
     <row r="141" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B141" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C141" s="44" t="str">
+      <c r="C141" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno10,CaléndárioMês10Opção+1,1),"mmmm")</f>
         <v>janeiro</v>
       </c>
-      <c r="D141" s="44"/>
-      <c r="E141" s="44"/>
+      <c r="D141" s="47"/>
+      <c r="E141" s="47"/>
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
       <c r="H141" s="2"/>
@@ -4847,23 +4798,23 @@
     <row r="154" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
-      <c r="D154" s="48"/>
-      <c r="E154" s="48"/>
-      <c r="F154" s="48"/>
-      <c r="G154" s="48"/>
-      <c r="H154" s="48"/>
+      <c r="D154" s="44"/>
+      <c r="E154" s="44"/>
+      <c r="F154" s="44"/>
+      <c r="G154" s="44"/>
+      <c r="H154" s="44"/>
     </row>
     <row r="155" spans="2:8" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B155" s="1">
         <f ca="1">YEAR(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1))</f>
         <v>2023</v>
       </c>
-      <c r="C155" s="44" t="str">
+      <c r="C155" s="47" t="str">
         <f ca="1">TEXT(DATE(CalendárioAno11,CaléndárioMês11Opção+1,1),"mmmm")</f>
         <v>fevereiro</v>
       </c>
-      <c r="D155" s="44"/>
-      <c r="E155" s="44"/>
+      <c r="D155" s="47"/>
+      <c r="E155" s="47"/>
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
       <c r="H155" s="2"/>
@@ -5113,14 +5064,34 @@
     <row r="168" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
-      <c r="D168" s="48"/>
-      <c r="E168" s="48"/>
-      <c r="F168" s="48"/>
-      <c r="G168" s="48"/>
-      <c r="H168" s="48"/>
+      <c r="D168" s="44"/>
+      <c r="E168" s="44"/>
+      <c r="F168" s="44"/>
+      <c r="G168" s="44"/>
+      <c r="H168" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="D83:H83"/>
+    <mergeCell ref="D153:H153"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D56:H56"/>
+    <mergeCell ref="D70:H70"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="D69:H69"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D41:H41"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C99:E99"/>
     <mergeCell ref="D168:H168"/>
     <mergeCell ref="D139:H139"/>
     <mergeCell ref="D140:H140"/>
@@ -5137,26 +5108,6 @@
     <mergeCell ref="C127:E127"/>
     <mergeCell ref="C141:E141"/>
     <mergeCell ref="C155:E155"/>
-    <mergeCell ref="D153:H153"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D56:H56"/>
-    <mergeCell ref="D70:H70"/>
-    <mergeCell ref="D55:H55"/>
-    <mergeCell ref="D69:H69"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="D83:H83"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">
@@ -5668,24 +5619,23 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AY9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="51" width="11.25" style="39" customWidth="1"/>
-    <col min="52" max="16384" width="9" style="39"/>
+    <col min="1" max="1" width="19.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="22" width="26.25" style="39" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="36" customFormat="1" ht="59.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="36" customFormat="1" ht="73.5" x14ac:dyDescent="0.3">
       <c r="A1" s="35"/>
       <c r="B1" s="35" t="s">
         <v>27</v>
@@ -5693,160 +5643,77 @@
       <c r="C1" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="H1" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="J1" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="K1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="L1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="M1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="N1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="O1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="P1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="R1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="S1" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="T1" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="U1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="V1" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="W1" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z1" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA1" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB1" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC1" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD1" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE1" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF1" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG1" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH1" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI1" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL1" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM1" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN1" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO1" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP1" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ1" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR1" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="AS1" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT1" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU1" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV1" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW1" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX1" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="AY1" s="35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+        <v>55</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>55</v>
+      </c>
       <c r="E2" s="38"/>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
@@ -5865,51 +5732,26 @@
       <c r="T2" s="38"/>
       <c r="U2" s="38"/>
       <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="38"/>
-      <c r="AE2" s="38"/>
-      <c r="AF2" s="38"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="38"/>
-      <c r="AM2" s="38"/>
-      <c r="AN2" s="38"/>
-      <c r="AO2" s="38"/>
-      <c r="AP2" s="38"/>
-      <c r="AQ2" s="38"/>
-      <c r="AR2" s="38"/>
-      <c r="AS2" s="38"/>
-      <c r="AT2" s="38"/>
-      <c r="AU2" s="38"/>
-      <c r="AV2" s="38"/>
-      <c r="AW2" s="38"/>
-      <c r="AX2" s="38"/>
-      <c r="AY2" s="38"/>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B3" s="40">
         <v>44675</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="38"/>
+      <c r="C3" s="40">
+        <v>44682</v>
+      </c>
+      <c r="D3" s="40">
+        <v>44682</v>
+      </c>
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="38"/>
       <c r="L3" s="38"/>
       <c r="M3" s="38"/>
@@ -5922,45 +5764,20 @@
       <c r="T3" s="38"/>
       <c r="U3" s="38"/>
       <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="38"/>
-      <c r="AE3" s="38"/>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="38"/>
-      <c r="AI3" s="38"/>
-      <c r="AJ3" s="38"/>
-      <c r="AK3" s="38"/>
-      <c r="AL3" s="38"/>
-      <c r="AM3" s="38"/>
-      <c r="AN3" s="38"/>
-      <c r="AO3" s="38"/>
-      <c r="AP3" s="38"/>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="38"/>
-      <c r="AS3" s="38"/>
-      <c r="AT3" s="38"/>
-      <c r="AU3" s="38"/>
-      <c r="AV3" s="38"/>
-      <c r="AW3" s="38"/>
-      <c r="AX3" s="38"/>
-      <c r="AY3" s="38"/>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="B4" s="38">
         <v>20</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="C4" s="38">
+        <v>20</v>
+      </c>
+      <c r="D4" s="38">
+        <v>20</v>
+      </c>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -5979,45 +5796,20 @@
       <c r="T4" s="38"/>
       <c r="U4" s="38"/>
       <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="38"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
-      <c r="AI4" s="38"/>
-      <c r="AJ4" s="38"/>
-      <c r="AK4" s="38"/>
-      <c r="AL4" s="38"/>
-      <c r="AM4" s="38"/>
-      <c r="AN4" s="38"/>
-      <c r="AO4" s="38"/>
-      <c r="AP4" s="38"/>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
-      <c r="AU4" s="38"/>
-      <c r="AV4" s="38"/>
-      <c r="AW4" s="38"/>
-      <c r="AX4" s="38"/>
-      <c r="AY4" s="38"/>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B5" s="38">
         <v>22</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+      <c r="C5" s="38">
+        <v>22</v>
+      </c>
+      <c r="D5" s="38">
+        <v>22</v>
+      </c>
       <c r="E5" s="38"/>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -6036,45 +5828,20 @@
       <c r="T5" s="38"/>
       <c r="U5" s="38"/>
       <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="38"/>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="38"/>
-      <c r="AI5" s="38"/>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="38"/>
-      <c r="AL5" s="38"/>
-      <c r="AM5" s="38"/>
-      <c r="AN5" s="38"/>
-      <c r="AO5" s="38"/>
-      <c r="AP5" s="38"/>
-      <c r="AQ5" s="38"/>
-      <c r="AR5" s="38"/>
-      <c r="AS5" s="38"/>
-      <c r="AT5" s="38"/>
-      <c r="AU5" s="38"/>
-      <c r="AV5" s="38"/>
-      <c r="AW5" s="38"/>
-      <c r="AX5" s="38"/>
-      <c r="AY5" s="38"/>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+        <v>57</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>57</v>
+      </c>
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
@@ -6093,45 +5860,20 @@
       <c r="T6" s="38"/>
       <c r="U6" s="38"/>
       <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="38"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="38"/>
-      <c r="AC6" s="38"/>
-      <c r="AD6" s="38"/>
-      <c r="AE6" s="38"/>
-      <c r="AF6" s="38"/>
-      <c r="AG6" s="38"/>
-      <c r="AH6" s="38"/>
-      <c r="AI6" s="38"/>
-      <c r="AJ6" s="38"/>
-      <c r="AK6" s="38"/>
-      <c r="AL6" s="38"/>
-      <c r="AM6" s="38"/>
-      <c r="AN6" s="38"/>
-      <c r="AO6" s="38"/>
-      <c r="AP6" s="38"/>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="38"/>
-      <c r="AS6" s="38"/>
-      <c r="AT6" s="38"/>
-      <c r="AU6" s="38"/>
-      <c r="AV6" s="38"/>
-      <c r="AW6" s="38"/>
-      <c r="AX6" s="38"/>
-      <c r="AY6" s="38"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="B7" s="43">
         <v>500</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="38">
+        <v>500</v>
+      </c>
+      <c r="D7" s="38">
+        <v>500</v>
+      </c>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
@@ -6150,45 +5892,20 @@
       <c r="T7" s="38"/>
       <c r="U7" s="38"/>
       <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
-      <c r="AC7" s="38"/>
-      <c r="AD7" s="38"/>
-      <c r="AE7" s="38"/>
-      <c r="AF7" s="38"/>
-      <c r="AG7" s="38"/>
-      <c r="AH7" s="38"/>
-      <c r="AI7" s="38"/>
-      <c r="AJ7" s="38"/>
-      <c r="AK7" s="38"/>
-      <c r="AL7" s="38"/>
-      <c r="AM7" s="38"/>
-      <c r="AN7" s="38"/>
-      <c r="AO7" s="38"/>
-      <c r="AP7" s="38"/>
-      <c r="AQ7" s="38"/>
-      <c r="AR7" s="38"/>
-      <c r="AS7" s="38"/>
-      <c r="AT7" s="38"/>
-      <c r="AU7" s="38"/>
-      <c r="AV7" s="38"/>
-      <c r="AW7" s="38"/>
-      <c r="AX7" s="38"/>
-      <c r="AY7" s="38"/>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="37" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+        <v>64</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>68</v>
+      </c>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -6207,45 +5924,20 @@
       <c r="T8" s="38"/>
       <c r="U8" s="38"/>
       <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-      <c r="Y8" s="38"/>
-      <c r="Z8" s="38"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
-      <c r="AC8" s="38"/>
-      <c r="AD8" s="38"/>
-      <c r="AE8" s="38"/>
-      <c r="AF8" s="38"/>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="38"/>
-      <c r="AI8" s="38"/>
-      <c r="AJ8" s="38"/>
-      <c r="AK8" s="38"/>
-      <c r="AL8" s="38"/>
-      <c r="AM8" s="38"/>
-      <c r="AN8" s="38"/>
-      <c r="AO8" s="38"/>
-      <c r="AP8" s="38"/>
-      <c r="AQ8" s="38"/>
-      <c r="AR8" s="38"/>
-      <c r="AS8" s="38"/>
-      <c r="AT8" s="38"/>
-      <c r="AU8" s="38"/>
-      <c r="AV8" s="38"/>
-      <c r="AW8" s="38"/>
-      <c r="AX8" s="38"/>
-      <c r="AY8" s="38"/>
-    </row>
-    <row r="9" spans="1:51" ht="231" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:22" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+        <v>63</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>67</v>
+      </c>
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
@@ -6264,35 +5956,6 @@
       <c r="T9" s="38"/>
       <c r="U9" s="38"/>
       <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="38"/>
-      <c r="AE9" s="38"/>
-      <c r="AF9" s="38"/>
-      <c r="AG9" s="38"/>
-      <c r="AH9" s="38"/>
-      <c r="AI9" s="38"/>
-      <c r="AJ9" s="38"/>
-      <c r="AK9" s="38"/>
-      <c r="AL9" s="38"/>
-      <c r="AM9" s="38"/>
-      <c r="AN9" s="38"/>
-      <c r="AO9" s="38"/>
-      <c r="AP9" s="38"/>
-      <c r="AQ9" s="38"/>
-      <c r="AR9" s="38"/>
-      <c r="AS9" s="38"/>
-      <c r="AT9" s="38"/>
-      <c r="AU9" s="38"/>
-      <c r="AV9" s="38"/>
-      <c r="AW9" s="38"/>
-      <c r="AX9" s="38"/>
-      <c r="AY9" s="38"/>
     </row>
   </sheetData>
   <phoneticPr fontId="27" type="noConversion"/>
@@ -6302,6 +5965,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="426e97fa315356fffbdcd9876fe988c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14b8f0def80e6d70ce3def20c90759ae" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -6522,25 +6203,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B0EC2F5-DB17-4B75-9677-570CB7A949FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6557,22 +6238,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F033DEB-E0CE-477C-A830-2CEC4FBEB4C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E064F5-287A-4749-B81B-14A9CFF48002}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>